<commit_message>
added balance sheet title in GOOGL model
</commit_message>
<xml_diff>
--- a/models/GOOGL.xlsx
+++ b/models/GOOGL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/257f0455a2bc8494/Documenten/Investing/Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\investing\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="8_{C3953DB9-6DE6-467C-87BD-0705897ABE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9112C09-2968-4CAA-9B99-8E46AD4C78B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA1B72-80D6-4B0A-817C-E6934F36F20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="744" windowWidth="30216" windowHeight="12120" activeTab="1" xr2:uid="{F618A5BB-0A8B-4542-9BE9-E604DC5354A7}"/>
+    <workbookView xWindow="11964" yWindow="0" windowWidth="7500" windowHeight="8040" activeTab="1" xr2:uid="{F618A5BB-0A8B-4542-9BE9-E604DC5354A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Price</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
   </si>
 </sst>
 </file>
@@ -737,13 +740,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAACBB6E-468B-4663-8256-54D95EF2727B}">
-  <dimension ref="B2:BU32"/>
+  <dimension ref="B2:BU35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,27 +983,27 @@
         <v>42337</v>
       </c>
       <c r="L5" s="2">
-        <f>+L3+L4</f>
+        <f t="shared" ref="L5:Q5" si="3">+L3+L4</f>
         <v>55134</v>
       </c>
       <c r="M5" s="2">
-        <f>+M3+M4</f>
+        <f t="shared" si="3"/>
         <v>65272</v>
       </c>
       <c r="N5" s="2">
-        <f>+N3+N4</f>
+        <f t="shared" si="3"/>
         <v>77270</v>
       </c>
       <c r="O5" s="2">
-        <f>+O3+O4</f>
+        <f t="shared" si="3"/>
         <v>89961</v>
       </c>
       <c r="P5" s="2">
-        <f>+P3+P4</f>
+        <f t="shared" si="3"/>
         <v>97785</v>
       </c>
       <c r="Q5" s="2">
-        <f>+Q3+Q4</f>
+        <f t="shared" si="3"/>
         <v>146698</v>
       </c>
     </row>
@@ -1191,27 +1194,27 @@
         <v>21885</v>
       </c>
       <c r="L9" s="2">
-        <f>+SUM(L5:L8)</f>
+        <f t="shared" ref="L9:Q9" si="4">+SUM(L5:L8)</f>
         <v>23716</v>
       </c>
       <c r="M9" s="2">
-        <f>+SUM(M5:M8)</f>
+        <f t="shared" si="4"/>
         <v>26146</v>
       </c>
       <c r="N9" s="2">
-        <f>+SUM(N5:N8)</f>
+        <f t="shared" si="4"/>
         <v>26321</v>
       </c>
       <c r="O9" s="2">
-        <f>+SUM(O5:O8)</f>
+        <f t="shared" si="4"/>
         <v>34231</v>
       </c>
       <c r="P9" s="2">
-        <f>+SUM(P5:P8)</f>
+        <f t="shared" si="4"/>
         <v>41214</v>
       </c>
       <c r="Q9" s="2">
-        <f>+SUM(Q5:Q8)</f>
+        <f t="shared" si="4"/>
         <v>78714</v>
       </c>
     </row>
@@ -1301,27 +1304,27 @@
         <v>24402</v>
       </c>
       <c r="L11" s="2">
-        <f>+L9+L10</f>
+        <f t="shared" ref="L11:Q11" si="5">+L9+L10</f>
         <v>24150</v>
       </c>
       <c r="M11" s="2">
-        <f>+M9+M10</f>
+        <f t="shared" si="5"/>
         <v>27193</v>
       </c>
       <c r="N11" s="2">
-        <f>+N9+N10</f>
+        <f t="shared" si="5"/>
         <v>34913</v>
       </c>
       <c r="O11" s="2">
-        <f>+O9+O10</f>
+        <f t="shared" si="5"/>
         <v>39625</v>
       </c>
       <c r="P11" s="2">
-        <f>+P9+P10</f>
+        <f t="shared" si="5"/>
         <v>48072</v>
       </c>
       <c r="Q11" s="2">
-        <f>+Q9+Q10</f>
+        <f t="shared" si="5"/>
         <v>90734</v>
       </c>
     </row>
@@ -1411,27 +1414,27 @@
         <v>20642</v>
       </c>
       <c r="L13" s="2">
-        <f>+L11+L12</f>
+        <f t="shared" ref="L13:Q13" si="6">+L11+L12</f>
         <v>19478</v>
       </c>
       <c r="M13" s="2">
-        <f>+M11+M12</f>
+        <f t="shared" si="6"/>
         <v>12662</v>
       </c>
       <c r="N13" s="2">
-        <f>+N11+N12</f>
+        <f t="shared" si="6"/>
         <v>30736</v>
       </c>
       <c r="O13" s="2">
-        <f>+O11+O12</f>
+        <f t="shared" si="6"/>
         <v>34343</v>
       </c>
       <c r="P13" s="2">
-        <f>+P11+P12</f>
+        <f t="shared" si="6"/>
         <v>40259</v>
       </c>
       <c r="Q13" s="2">
-        <f>+Q11+Q12</f>
+        <f t="shared" si="6"/>
         <v>76033</v>
       </c>
       <c r="R13" s="2">
@@ -1439,19 +1442,19 @@
         <v>81355.31</v>
       </c>
       <c r="S13" s="2">
-        <f t="shared" ref="S13:W13" si="3">+R13*(1+$C$28)</f>
+        <f t="shared" ref="S13:V13" si="7">+R13*(1+$C$28)</f>
         <v>87050.181700000001</v>
       </c>
       <c r="T13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>93143.694419000007</v>
       </c>
       <c r="U13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>99663.753028330015</v>
       </c>
       <c r="V13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>106640.21574031313</v>
       </c>
       <c r="W13" s="2">
@@ -1459,19 +1462,19 @@
         <v>110905.82436992566</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" ref="X13:AB13" si="4">+W13*(1+$D$28)</f>
+        <f t="shared" ref="X13:AA13" si="8">+W13*(1+$D$28)</f>
         <v>115342.05734472269</v>
       </c>
       <c r="Y13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>119955.7396385116</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>124753.96922405207</v>
       </c>
       <c r="AA13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>129744.12799301416</v>
       </c>
       <c r="AB13" s="2">
@@ -1479,183 +1482,183 @@
         <v>132339.01055287445</v>
       </c>
       <c r="AC13" s="2">
-        <f t="shared" ref="AC13:BU13" si="5">+AB13*(1+$E$28)</f>
+        <f t="shared" ref="AC13:BU13" si="9">+AB13*(1+$E$28)</f>
         <v>134985.79076393193</v>
       </c>
       <c r="AD13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>137685.50657921057</v>
       </c>
       <c r="AE13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>140439.21671079478</v>
       </c>
       <c r="AF13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>143248.00104501066</v>
       </c>
       <c r="AG13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>146112.96106591087</v>
       </c>
       <c r="AH13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>149035.22028722908</v>
       </c>
       <c r="AI13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>152015.92469297367</v>
       </c>
       <c r="AJ13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>155056.24318683313</v>
       </c>
       <c r="AK13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>158157.36805056978</v>
       </c>
       <c r="AL13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>161320.51541158117</v>
       </c>
       <c r="AM13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>164546.9257198128</v>
       </c>
       <c r="AN13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>167837.86423420906</v>
       </c>
       <c r="AO13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>171194.62151889325</v>
       </c>
       <c r="AP13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>174618.51394927112</v>
       </c>
       <c r="AQ13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>178110.88422825653</v>
       </c>
       <c r="AR13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>181673.10191282167</v>
       </c>
       <c r="AS13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>185306.5639510781</v>
       </c>
       <c r="AT13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>189012.69523009966</v>
       </c>
       <c r="AU13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>192792.94913470166</v>
       </c>
       <c r="AV13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>196648.8081173957</v>
       </c>
       <c r="AW13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>200581.78427974362</v>
       </c>
       <c r="AX13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>204593.41996533849</v>
       </c>
       <c r="AY13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>208685.28836464527</v>
       </c>
       <c r="AZ13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>212858.99413193818</v>
       </c>
       <c r="BA13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>217116.17401457694</v>
       </c>
       <c r="BB13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>221458.4974948685</v>
       </c>
       <c r="BC13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>225887.66744476586</v>
       </c>
       <c r="BD13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>230405.42079366118</v>
       </c>
       <c r="BE13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>235013.5292095344</v>
       </c>
       <c r="BF13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>239713.79979372511</v>
       </c>
       <c r="BG13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>244508.07578959962</v>
       </c>
       <c r="BH13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>249398.23730539161</v>
       </c>
       <c r="BI13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>254386.20205149945</v>
       </c>
       <c r="BJ13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>259473.92609252944</v>
       </c>
       <c r="BK13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>264663.40461438004</v>
       </c>
       <c r="BL13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>269956.67270666762</v>
       </c>
       <c r="BM13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>275355.80616080097</v>
       </c>
       <c r="BN13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>280862.92228401703</v>
       </c>
       <c r="BO13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>286480.1807296974</v>
       </c>
       <c r="BP13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>292209.78434429137</v>
       </c>
       <c r="BQ13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>298053.98003117723</v>
       </c>
       <c r="BR13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>304015.0596318008</v>
       </c>
       <c r="BS13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>310095.36082443682</v>
       </c>
       <c r="BT13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>316297.26804092556</v>
       </c>
       <c r="BU13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>322623.21340174408</v>
       </c>
     </row>
@@ -1664,15 +1667,15 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:E15" si="6">300.737081+45.843112+327.556472</f>
+        <f t="shared" ref="C15:E15" si="10">300.737081+45.843112+327.556472</f>
         <v>674.13666499999999</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>674.13666499999999</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>674.13666499999999</v>
       </c>
       <c r="F15" s="1">
@@ -1725,59 +1728,59 @@
         <v>18</v>
       </c>
       <c r="C16" s="3">
-        <f>+C13/C15</f>
+        <f t="shared" ref="C16:J16" si="11">+C13/C15</f>
         <v>10.140377099946047</v>
       </c>
       <c r="D16" s="3">
-        <f>+D13/D15</f>
+        <f t="shared" si="11"/>
         <v>10.322832685565322</v>
       </c>
       <c r="E16" s="3">
-        <f>+E13/E15</f>
+        <f t="shared" si="11"/>
         <v>16.683560743577122</v>
       </c>
       <c r="F16" s="3">
-        <f>+F13/F15</f>
+        <f t="shared" si="11"/>
         <v>22.572574360719575</v>
       </c>
       <c r="G16" s="3">
-        <f>+G13/G15</f>
+        <f t="shared" si="11"/>
         <v>26.754653395606528</v>
       </c>
       <c r="H16" s="3">
-        <f>+H13/H15</f>
+        <f t="shared" si="11"/>
         <v>27.78382264437008</v>
       </c>
       <c r="I16" s="3">
-        <f>+I13/I15</f>
+        <f t="shared" si="11"/>
         <v>28.528212092203361</v>
       </c>
       <c r="J16" s="3">
-        <f>+J13/J15</f>
+        <f t="shared" si="11"/>
         <v>31.229797203709495</v>
       </c>
       <c r="L16" s="3">
-        <f>+L13/L15</f>
+        <f t="shared" ref="L16:Q16" si="12">+L13/L15</f>
         <v>28.013906507045981</v>
       </c>
       <c r="M16" s="3">
-        <f>+M13/M15</f>
+        <f t="shared" si="12"/>
         <v>18.213820168022963</v>
       </c>
       <c r="N16" s="3">
-        <f>+N13/N15</f>
+        <f t="shared" si="12"/>
         <v>44.212602802428826</v>
       </c>
       <c r="O16" s="3">
-        <f>+O13/O15</f>
+        <f t="shared" si="12"/>
         <v>49.969001991586936</v>
       </c>
       <c r="P16" s="3">
-        <f>+P13/P15</f>
+        <f t="shared" si="12"/>
         <v>59.719344889808063</v>
       </c>
       <c r="Q16" s="3">
-        <f>+Q13/Q15</f>
+        <f t="shared" si="12"/>
         <v>115.03222414444551</v>
       </c>
     </row>
@@ -1790,47 +1793,47 @@
         <v>-6.9535217084963241E-2</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" ref="E18:J18" si="7">+E3/D3-1</f>
+        <f t="shared" ref="E18:J18" si="13">+E3/D3-1</f>
         <v>0.20565579549311952</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.23206202759188277</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>-2.7668401068766668E-2</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.11870412553783849</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>5.2327084680025893E-2</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.15674621456432947</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" ref="L18:Q18" si="8">+M3/L3-1</f>
+        <f t="shared" ref="M18:Q18" si="14">+M3/L3-1</f>
         <v>0.22801090038993266</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.23421586757475987</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.18300089899794614</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.12764353719641419</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.41157809957428615</v>
       </c>
     </row>
@@ -1843,55 +1846,55 @@
         <v>0.53881289632887097</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" ref="D20:J20" si="9">+D5/D3</f>
+        <f t="shared" ref="D20:J20" si="15">+D5/D3</f>
         <v>0.51554952085019712</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.54265479825872265</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.54155533680213752</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.56425136493473627</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.57616354234001288</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.57583156730857832</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.56205774975107869</v>
       </c>
       <c r="L20" s="4">
-        <f t="shared" ref="L20:Q20" si="10">+L5/L3</f>
+        <f t="shared" ref="L20:Q20" si="16">+L5/L3</f>
         <v>0.61075416518964909</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.58880519597672631</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.5647607422945643</v>
       </c>
       <c r="O20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.5558054331910266</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.53575831292427556</v>
       </c>
       <c r="Q20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.5693980290098084</v>
       </c>
     </row>
@@ -1904,55 +1907,55 @@
         <v>0.1938093734055735</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" ref="D21:J21" si="11">+D9/D3</f>
+        <f t="shared" ref="D21:J21" si="17">+D9/D3</f>
         <v>0.1666710186176463</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.24284755159941956</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.27494374912107999</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.29715804317171057</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.312879767291532</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.32296753585798088</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.29054098904746101</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" ref="L21:Q21" si="12">+L9/L3</f>
+        <f t="shared" ref="L21:Q21" si="18">+L9/L3</f>
         <v>0.26271712158808935</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.23585765188760091</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.19237825155862856</v>
       </c>
       <c r="O21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.21148915400631421</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.22580910271371982</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.3055228868524319</v>
       </c>
     </row>
@@ -1965,55 +1968,55 @@
         <v>0.16608761145800433</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:J22" si="13">+D13/D3</f>
+        <f t="shared" ref="D22:J22" si="19">+D13/D3</f>
         <v>0.1817113612032274</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.24358391267623936</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.26749050766418225</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.32414940159814876</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.29936974789915966</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.29079517184188702</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0.2740391636242947</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" ref="L22:Q22" si="14">+L13/L3</f>
+        <f t="shared" ref="L22:Q22" si="20">+L13/L3</f>
         <v>0.2157701169797944</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.11422128005051645</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.22464716157843576</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.21218112284300339</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.22057671340203927</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.29511677282377918</v>
       </c>
     </row>
@@ -2026,27 +2029,27 @@
         <v>0.11873146835116669</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" ref="D23:J23" si="15">ABS(D12/D11)</f>
+        <f t="shared" ref="D23:I23" si="21">ABS(D12/D11)</f>
         <v>0.15923643832306392</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.15809566584325174</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.18534182772097008</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.15754357938260583</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.15738003183989083</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.17898022892819979</v>
       </c>
       <c r="J23" s="4">
@@ -2054,27 +2057,27 @@
         <v>0.15408573067781328</v>
       </c>
       <c r="L23" s="4">
-        <f t="shared" ref="L23:Q23" si="16">ABS(L12/L11)</f>
+        <f t="shared" ref="L23:Q23" si="22">ABS(L12/L11)</f>
         <v>0.19345755693581781</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.53436546169970212</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.1196402486179933</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.13329968454258675</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.16252704276917956</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.16202305640663919</v>
       </c>
     </row>
@@ -2151,6 +2154,11 @@
       <c r="C32" s="1">
         <f>+C31-C25</f>
         <v>950.62354061593078</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>